<commit_message>
Cronbach alpha + Bland-Altman
</commit_message>
<xml_diff>
--- a/data/Wearable Inertial Sensors for Exergames (post survey)_August 31, 2019_11.58.xlsx
+++ b/data/Wearable Inertial Sensors for Exergames (post survey)_August 31, 2019_11.58.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\github\wearable-jacket\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E170883-8FC9-4DAF-9E7F-7F81D89D6A5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF11F825-D8E2-4B4D-B1AF-CA3F00884BBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="612" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="175">
   <si>
     <t>StartDate</t>
   </si>
@@ -553,6 +553,36 @@
   </si>
   <si>
     <t>C alpha</t>
+  </si>
+  <si>
+    <t>SID</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>Q8</t>
+  </si>
+  <si>
+    <t>Sum of scores</t>
+  </si>
+  <si>
+    <t>Var of scores</t>
   </si>
 </sst>
 </file>
@@ -1090,7 +1120,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1144,6 +1174,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1272,7 +1305,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5481A1F5-40FC-4BB1-BED1-E332D1461A6C}" type="CELLRANGE">
+                    <a:fld id="{0EE18808-2F9A-4EBC-80A2-5AB9E45E94AA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1305,7 +1338,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B15E3A1A-32C1-46D5-B0B2-11EDB296D58C}" type="CELLRANGE">
+                    <a:fld id="{7EF09159-3539-4327-9370-ACCC93FF1C53}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1339,7 +1372,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B8E510BB-C56D-430D-9150-9FA96640C120}" type="CELLRANGE">
+                    <a:fld id="{430ACAF1-286A-4DBB-A307-D45568CAAE81}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1373,7 +1406,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{84ACB996-1CE6-4926-8B9B-2F6AF806AD9F}" type="CELLRANGE">
+                    <a:fld id="{73EF237C-E46D-49FB-8005-71B3F0E2B90E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1413,7 +1446,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{95E82AE1-F149-4F6B-B515-E714F5EB8F1C}" type="CELLRANGE">
+                    <a:fld id="{2DC3080C-CB4C-427E-B5A3-5C212209E818}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1446,7 +1479,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{12583016-FAA0-426E-AC6F-47F8A72C5077}" type="CELLRANGE">
+                    <a:fld id="{DA240189-E3B8-4BE0-8F76-3856F7FB18E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1480,7 +1513,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CA892C44-ABF4-4CB0-A6AD-BD871AAE72B7}" type="CELLRANGE">
+                    <a:fld id="{68521C6F-03C5-42F3-B34B-A4A65014C442}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1520,7 +1553,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{39AC322B-D414-4295-8519-5A2F4303F9CC}" type="CELLRANGE">
+                    <a:fld id="{055E07E0-8347-425D-A3FC-D54402F68DFE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1553,7 +1586,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{28C91C74-FBF4-4989-8BC5-11B61F5C5E90}" type="CELLRANGE">
+                    <a:fld id="{0AFF8321-1931-4F1D-BE13-C7C2D832A56B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1587,7 +1620,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D157F1A-AE82-4D80-AF63-FDB3070D0D42}" type="CELLRANGE">
+                    <a:fld id="{532173A4-C7B3-45E7-8B57-26DDCEFFB499}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1805,7 +1838,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AFA2F518-4E73-4CCA-AF9E-FC8E6949CAB3}" type="CELLRANGE">
+                    <a:fld id="{DE9E62CD-FC3B-498C-B4F7-1416DA691BCF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1838,7 +1871,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A2295B06-0778-4F5C-87FB-50AC67FA05FE}" type="CELLRANGE">
+                    <a:fld id="{B35974E9-ACA2-4C5A-9C6A-4009B8DD35EA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1872,7 +1905,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C3D1BA42-69E7-41FE-8D42-96DCB8334775}" type="CELLRANGE">
+                    <a:fld id="{6FF9F3A2-AAEF-4075-8974-B19B5E7C39E3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1906,7 +1939,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{507609C0-DABB-4D5F-9E6B-8956172109A4}" type="CELLRANGE">
+                    <a:fld id="{23116A68-313B-423C-94D5-1835928376BA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1940,7 +1973,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F15C35E0-9CB0-4F0B-B3A5-0EFFA728D8E9}" type="CELLRANGE">
+                    <a:fld id="{CB710C7B-E5A3-452B-9CD3-532F61038CA2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1974,7 +2007,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5691EE09-D80F-4D55-ABBD-7C47F6A0D4F4}" type="CELLRANGE">
+                    <a:fld id="{CDCA02FE-BA9C-42A3-A79B-121B990E7C83}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2008,7 +2041,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F29B75A5-7C0C-46DB-8A5A-C4893709D4F5}" type="CELLRANGE">
+                    <a:fld id="{57293735-A599-480A-8161-F3C1AF6FCDA5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2042,7 +2075,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5687B16E-F5D4-43D9-9F62-842D8F579CB8}" type="CELLRANGE">
+                    <a:fld id="{69FBE8F8-5C2A-406A-A27F-FE20DF8C10FE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2076,7 +2109,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CF33A2BD-9DF5-4D9A-9079-C51E69E7B8E9}" type="CELLRANGE">
+                    <a:fld id="{1647A1F7-CC1F-4375-BB9B-28FFE09F65AD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2110,7 +2143,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EAA775FB-A97E-4591-848A-B694487BD740}" type="CELLRANGE">
+                    <a:fld id="{8788A963-F285-4868-B4DD-9DC898E52864}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2337,7 +2370,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5D8ABEF1-1044-4A28-B994-3468E8E7337B}" type="CELLRANGE">
+                    <a:fld id="{3BD1EEF2-2745-45E3-AFE3-4B6BFA076509}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2371,7 +2404,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E39B32FF-DD7B-40B4-A1A9-4CC4ECE90B95}" type="CELLRANGE">
+                    <a:fld id="{553864B7-533D-47CD-9C9C-56616163EEFD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2405,7 +2438,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{15ABA255-3FCA-4CC3-8B99-FBD94BB732A4}" type="CELLRANGE">
+                    <a:fld id="{57306957-B7B7-4F09-A25B-9C5F1FD74FB9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2439,7 +2472,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4A375B5B-AE04-4156-AE80-1054D476155B}" type="CELLRANGE">
+                    <a:fld id="{EA8C31DD-5694-476F-BB2B-64D1C98CECD1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2473,7 +2506,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD8011A5-F5D3-49AC-A96B-87AFD59B7DDC}" type="CELLRANGE">
+                    <a:fld id="{B9B49668-81D0-41E6-8300-5D8051322150}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2507,7 +2540,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{935CF20F-AF1E-4C17-B0D9-0C72BDB4B405}" type="CELLRANGE">
+                    <a:fld id="{AD280660-8009-449F-836B-4AC10E1E6C04}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2541,7 +2574,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3C32470A-CCFB-4E88-AA3F-346D9CA31A62}" type="CELLRANGE">
+                    <a:fld id="{DF4FA372-8ED5-45BC-BBD8-4FAE20A0AE4B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2575,7 +2608,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{393D5326-F756-4C33-8267-A4FB4DEC0DE4}" type="CELLRANGE">
+                    <a:fld id="{7F35CB66-412D-47E5-A5C9-BCBE59B96EB6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2609,7 +2642,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F7BA365E-3A4D-4052-8F16-81207F8887AE}" type="CELLRANGE">
+                    <a:fld id="{A6C9F675-9FD4-4AA6-A1E7-C0D241B575F6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2643,7 +2676,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BB72FF73-8F4E-46E5-A477-69E6FF7FFD9C}" type="CELLRANGE">
+                    <a:fld id="{2F1D3B5D-362A-4032-B5D4-79BB62294558}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2977,7 +3010,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D394C2EB-725A-4DD7-B358-5E9B3F3AC3AC}" type="CELLRANGE">
+                    <a:fld id="{72FBFEC3-7771-4536-842E-5A084DA281E2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3011,7 +3044,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{63EE8E22-F2B7-4DBD-B6B7-576E4F997DB2}" type="CELLRANGE">
+                    <a:fld id="{5D58C99F-C2BD-4576-BB1E-9816C0B6B4E8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3045,7 +3078,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{27C5B4FD-D8F2-47BD-B406-B86242653F79}" type="CELLRANGE">
+                    <a:fld id="{1B6F112B-86CC-4573-909B-36F83EBB5293}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3079,7 +3112,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F54459D6-4FE7-4674-9C6E-7847087D5BAC}" type="CELLRANGE">
+                    <a:fld id="{424285C5-F7D6-4B10-B9D5-D292FC53C554}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3113,7 +3146,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{33D7CF64-C8BC-412A-BD9D-AD76ED0353D8}" type="CELLRANGE">
+                    <a:fld id="{D23FAFC4-956A-482A-8C9C-44917C28CD3F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3147,7 +3180,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A3CC3A73-E23E-4284-9C38-EB7650F240A0}" type="CELLRANGE">
+                    <a:fld id="{428FF211-1B59-4E79-A384-7987E8E951BE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3181,7 +3214,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{73A95AC8-5377-42CB-A397-8EDA1ECDB746}" type="CELLRANGE">
+                    <a:fld id="{D84AFA1D-EDF4-43BC-84D2-A5E94441706E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3215,7 +3248,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D2148BF8-5657-44B0-8AF8-B1A2ED08AF3F}" type="CELLRANGE">
+                    <a:fld id="{EAE99573-3B57-4021-A063-66B517EF1114}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3249,7 +3282,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4AA76298-0186-45B4-B365-4EC71EE46A59}" type="CELLRANGE">
+                    <a:fld id="{5B3B4728-FB1D-4122-B95C-AFEF3DE483DA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3283,7 +3316,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7C4AF96-FCF4-44CA-82F5-694DA7E09096}" type="CELLRANGE">
+                    <a:fld id="{BE70C978-4873-484E-B6C1-0A48F2171FB6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3516,7 +3549,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{560B624F-8FEC-451E-BB6E-64F3ABAEE6F8}" type="CELLRANGE">
+                    <a:fld id="{07C887BA-733C-4A19-A5CD-9C7C8605602D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3550,7 +3583,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D513796B-E259-4C3E-AC36-434E0A3459F3}" type="CELLRANGE">
+                    <a:fld id="{9BA4C6EB-1CEF-4285-9B52-61E469E96B8F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3584,7 +3617,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{85290813-7C27-4111-B0C2-09EBB200BFCF}" type="CELLRANGE">
+                    <a:fld id="{B431E305-2443-496D-9F82-86648684E24F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3618,7 +3651,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{295CCC44-80F0-4859-870F-C2525DC3E064}" type="CELLRANGE">
+                    <a:fld id="{471B020D-82A3-4F20-B572-73D289D59AEE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3652,7 +3685,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ACCB2E74-CF82-48CB-AE3C-3747732A8EEA}" type="CELLRANGE">
+                    <a:fld id="{17BA4E8A-CC2A-4DFD-9B55-EA627A90830B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3686,7 +3719,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{909CF359-8770-4321-B31B-1D1D582FF7E7}" type="CELLRANGE">
+                    <a:fld id="{E9AE5BE1-4F88-455E-9C4E-479296A571B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3720,7 +3753,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB99D7E4-C287-4F7B-8671-6F0A35EAE19D}" type="CELLRANGE">
+                    <a:fld id="{F47326D2-D875-4770-88CE-07804168A4C9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3754,7 +3787,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{03191791-3373-4163-8A40-AD5612E0D58C}" type="CELLRANGE">
+                    <a:fld id="{2DE277FE-4F62-4466-9F31-6FFBF5F7CA1F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3788,7 +3821,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{656E7940-8B77-4513-ACE6-6DFBB44C9598}" type="CELLRANGE">
+                    <a:fld id="{44EA7E48-6F8A-497B-B34F-B383DE80A765}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3822,7 +3855,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F9CC8229-1EAC-446F-833F-0ACE82015780}" type="CELLRANGE">
+                    <a:fld id="{B3D9C25C-5A14-4ECF-9F1A-59F8231DFEC6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4211,7 +4244,7 @@
           <c:x val="4.0375683617569776E-2"/>
           <c:y val="3.9960035768951706E-2"/>
           <c:w val="0.91924863276486046"/>
-          <c:h val="0.85023298111349432"/>
+          <c:h val="0.86504357124013098"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -4248,7 +4281,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="8.78368751651264E-3"/>
-                  <c:y val="-"/>
+                  <c:y val="0"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -4312,7 +4345,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="1.4639479194187628E-2"/>
-                  <c:y val="-"/>
+                  <c:y val="0"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -4510,7 +4543,7 @@
             <c:numRef>
               <c:f>Sheet1!$AS$6:$AS$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>-5.882352941176471</c:v>
@@ -4711,7 +4744,7 @@
             <c:numRef>
               <c:f>Sheet1!$AT$6:$AT$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>-5.882352941176471</c:v>
@@ -4912,7 +4945,7 @@
             <c:numRef>
               <c:f>Sheet1!$AU$6:$AU$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -5022,7 +5055,7 @@
             <c:numRef>
               <c:f>Sheet1!$AV$6:$AV$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>5.882352941176471</c:v>
@@ -5243,7 +5276,7 @@
             <c:numRef>
               <c:f>Sheet1!$AW$6:$AW$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>47.058823529411768</c:v>
@@ -5444,7 +5477,7 @@
             <c:numRef>
               <c:f>Sheet1!$AX$6:$AX$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>35.294117647058826</c:v>
@@ -5576,8 +5609,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.0864995181387451E-2"/>
-          <c:y val="0.94388069132114694"/>
+          <c:x val="2.0864946539388498E-2"/>
+          <c:y val="0.95210882418034071"/>
           <c:w val="0.96141826021747279"/>
           <c:h val="3.8590534670987428E-2"/>
         </c:manualLayout>
@@ -5652,6 +5685,881 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$BW$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Strongly disagree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$BV$3:$BV$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>q4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>q5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>q6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>q7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>q8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>q9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>q10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$BW$3:$BW$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-76.470588235294116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-64.705882352941174</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.882352941176471</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-64.705882352941174</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-70.588235294117652</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-76.470588235294116</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9551-4833-9196-9C4451822367}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$BX$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Somewhat disagree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$BV$3:$BV$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>q4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>q5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>q6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>q7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>q8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>q9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>q10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$BX$3:$BX$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-5.882352941176471</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-23.529411764705884</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-17.647058823529413</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-23.529411764705884</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-23.529411764705884</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-17.647058823529413</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9551-4833-9196-9C4451822367}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$BY$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Neither agree nor disagree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$BV$3:$BV$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>q4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>q5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>q6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>q7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>q8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>q9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>q10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$BY$3:$BY$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-5.882352941176471</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.882352941176471</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2.9411764705882355</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9551-4833-9196-9C4451822367}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$BZ$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Neither agree nor disagree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$BV$3:$BV$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>q4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>q5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>q6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>q7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>q8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>q9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>q10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$BZ$3:$BZ$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5.882352941176471</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.882352941176471</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.9411764705882355</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9551-4833-9196-9C4451822367}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$CA$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Somewhat agree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$BV$3:$BV$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>q4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>q5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>q6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>q7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>q8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>q9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>q10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$CA$3:$CA$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>47.058823529411768</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.647058823529413</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.764705882352942</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.411764705882351</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.764705882352942</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.529411764705884</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.764705882352942</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.882352941176471</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-9551-4833-9196-9C4451822367}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$CB$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Strongly agree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$BV$3:$BV$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>q2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>q3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>q4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>q5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>q6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>q7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>q8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>q9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>q10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$CB$3:$CB$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>35.294117647058826</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82.352941176470594</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.882352941176471</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>52.941176470588232</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>76.470588235294116</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>88.235294117647058</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-9551-4833-9196-9C4451822367}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="650612735"/>
+        <c:axId val="649245951"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="650612735"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="649245951"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="649245951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="650612735"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5693,6 +6601,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6742,6 +7690,511 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6902,6 +8355,42 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>73</xdr:col>
+      <xdr:colOff>138544</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>50965</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>80</xdr:col>
+      <xdr:colOff>395843</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>160812</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF524EE4-98F9-47A1-8F31-8D79A627C1E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -11346,8 +12835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21BC5C2A-44C9-4F92-A0A1-E5355093D816}">
   <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12684,10 +14173,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2DD505A-8013-4D07-9F70-FBD34166A50F}">
-  <dimension ref="B1:AX37"/>
+  <dimension ref="B1:CB37"/>
   <sheetViews>
-    <sheetView topLeftCell="AN1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="BR16" sqref="BR16"/>
+    <sheetView topLeftCell="N35" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="V81" sqref="V81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12711,9 +14200,16 @@
     <col min="48" max="48" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:80" x14ac:dyDescent="0.25">
       <c r="AE1" t="s">
         <v>104</v>
       </c>
@@ -12733,7 +14229,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>137</v>
       </c>
@@ -12785,8 +14281,27 @@
       <c r="AJ2" s="3">
         <v>35.294117647058826</v>
       </c>
-    </row>
-    <row r="3" spans="2:50" x14ac:dyDescent="0.25">
+      <c r="BV2" s="2"/>
+      <c r="BW2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="BX2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="BY2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="CA2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="CB2" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>4</v>
       </c>
@@ -12868,8 +14383,29 @@
       <c r="AJ3" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:50" x14ac:dyDescent="0.25">
+      <c r="BV3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BW3" s="20">
+        <v>0</v>
+      </c>
+      <c r="BX3" s="20">
+        <v>-5.882352941176471</v>
+      </c>
+      <c r="BY3" s="20">
+        <v>-5.882352941176471</v>
+      </c>
+      <c r="BZ3" s="20">
+        <v>5.882352941176471</v>
+      </c>
+      <c r="CA3" s="20">
+        <v>47.058823529411768</v>
+      </c>
+      <c r="CB3" s="20">
+        <v>35.294117647058826</v>
+      </c>
+    </row>
+    <row r="4" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>4</v>
       </c>
@@ -12967,8 +14503,29 @@
       <c r="AJ4" s="3">
         <v>82.352941176470594</v>
       </c>
-    </row>
-    <row r="5" spans="2:50" x14ac:dyDescent="0.25">
+      <c r="BV4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="BW4" s="20">
+        <v>-76.470588235294116</v>
+      </c>
+      <c r="BX4" s="20">
+        <v>-23.529411764705884</v>
+      </c>
+      <c r="BY4" s="20">
+        <v>0</v>
+      </c>
+      <c r="BZ4" s="20">
+        <v>0</v>
+      </c>
+      <c r="CA4" s="20">
+        <v>0</v>
+      </c>
+      <c r="CB4" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>5</v>
       </c>
@@ -13066,26 +14623,48 @@
       <c r="AJ5" s="3">
         <v>5.882352941176471</v>
       </c>
-      <c r="AS5" t="s">
+      <c r="AR5" s="2"/>
+      <c r="AS5" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="AT5" t="s">
+      <c r="AT5" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="AU5" t="s">
+      <c r="AU5" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="AV5" t="s">
+      <c r="AV5" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AW5" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="AX5" t="s">
+      <c r="AX5" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="6" spans="2:50" x14ac:dyDescent="0.25">
+      <c r="BV5" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="BW5" s="20">
+        <v>0</v>
+      </c>
+      <c r="BX5" s="20">
+        <v>0</v>
+      </c>
+      <c r="BY5" s="20">
+        <v>0</v>
+      </c>
+      <c r="BZ5" s="20">
+        <v>0</v>
+      </c>
+      <c r="CA5" s="20">
+        <v>17.647058823529413</v>
+      </c>
+      <c r="CB5" s="20">
+        <v>82.352941176470594</v>
+      </c>
+    </row>
+    <row r="6" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
@@ -13183,29 +14762,50 @@
       <c r="AJ6" s="3">
         <v>52.941176470588232</v>
       </c>
-      <c r="AR6" t="s">
+      <c r="AR6" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="AS6">
+      <c r="AS6" s="20">
         <v>-5.882352941176471</v>
       </c>
-      <c r="AT6">
+      <c r="AT6" s="20">
         <v>-5.882352941176471</v>
       </c>
-      <c r="AU6">
+      <c r="AU6" s="20">
         <v>0</v>
       </c>
-      <c r="AV6">
+      <c r="AV6" s="20">
         <v>5.882352941176471</v>
       </c>
-      <c r="AW6">
+      <c r="AW6" s="20">
         <v>47.058823529411768</v>
       </c>
-      <c r="AX6">
+      <c r="AX6" s="20">
         <v>35.294117647058826</v>
       </c>
-    </row>
-    <row r="7" spans="2:50" x14ac:dyDescent="0.25">
+      <c r="BV6" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BW6" s="20">
+        <v>-64.705882352941174</v>
+      </c>
+      <c r="BX6" s="20">
+        <v>-17.647058823529413</v>
+      </c>
+      <c r="BY6" s="20">
+        <v>0</v>
+      </c>
+      <c r="BZ6" s="20">
+        <v>0</v>
+      </c>
+      <c r="CA6" s="20">
+        <v>11.764705882352942</v>
+      </c>
+      <c r="CB6" s="20">
+        <v>5.882352941176471</v>
+      </c>
+    </row>
+    <row r="7" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>3</v>
       </c>
@@ -13303,29 +14903,50 @@
       <c r="AJ7" s="3">
         <v>0</v>
       </c>
-      <c r="AR7" t="s">
+      <c r="AR7" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="AS7">
+      <c r="AS7" s="20">
         <v>0</v>
       </c>
-      <c r="AT7">
+      <c r="AT7" s="20">
         <v>-23.529411764705884</v>
       </c>
-      <c r="AU7">
+      <c r="AU7" s="20">
         <v>-76.470588235294116</v>
       </c>
-      <c r="AV7">
+      <c r="AV7" s="20">
         <v>0</v>
       </c>
-      <c r="AW7">
+      <c r="AW7" s="20">
         <v>0</v>
       </c>
-      <c r="AX7">
+      <c r="AX7" s="20">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:50" x14ac:dyDescent="0.25">
+      <c r="BV7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="BW7" s="20">
+        <v>-5.882352941176471</v>
+      </c>
+      <c r="BX7" s="20">
+        <v>0</v>
+      </c>
+      <c r="BY7" s="20">
+        <v>-5.882352941176471</v>
+      </c>
+      <c r="BZ7" s="20">
+        <v>5.882352941176471</v>
+      </c>
+      <c r="CA7" s="20">
+        <v>29.411764705882351</v>
+      </c>
+      <c r="CB7" s="20">
+        <v>52.941176470588232</v>
+      </c>
+    </row>
+    <row r="8" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>4</v>
       </c>
@@ -13423,29 +15044,50 @@
       <c r="AJ8" s="3">
         <v>76.470588235294116</v>
       </c>
-      <c r="AR8" t="s">
+      <c r="AR8" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="AS8">
+      <c r="AS8" s="20">
         <v>0</v>
       </c>
-      <c r="AT8">
+      <c r="AT8" s="20">
         <v>0</v>
       </c>
-      <c r="AU8">
+      <c r="AU8" s="20">
         <v>0</v>
       </c>
-      <c r="AV8">
+      <c r="AV8" s="20">
         <v>0</v>
       </c>
-      <c r="AW8">
+      <c r="AW8" s="20">
         <v>17.647058823529413</v>
       </c>
-      <c r="AX8">
+      <c r="AX8" s="20">
         <v>82.352941176470594</v>
       </c>
-    </row>
-    <row r="9" spans="2:50" x14ac:dyDescent="0.25">
+      <c r="BV8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="BW8" s="20">
+        <v>-64.705882352941174</v>
+      </c>
+      <c r="BX8" s="20">
+        <v>-23.529411764705884</v>
+      </c>
+      <c r="BY8" s="20">
+        <v>0</v>
+      </c>
+      <c r="BZ8" s="20">
+        <v>0</v>
+      </c>
+      <c r="CA8" s="20">
+        <v>11.764705882352942</v>
+      </c>
+      <c r="CB8" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2</v>
       </c>
@@ -13497,29 +15139,50 @@
       <c r="AJ9" s="3">
         <v>0</v>
       </c>
-      <c r="AR9" t="s">
+      <c r="AR9" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="AS9">
+      <c r="AS9" s="20">
         <v>0</v>
       </c>
-      <c r="AT9">
+      <c r="AT9" s="20">
         <v>-17.647058823529413</v>
       </c>
-      <c r="AU9">
+      <c r="AU9" s="20">
         <v>-64.705882352941174</v>
       </c>
-      <c r="AV9">
+      <c r="AV9" s="20">
         <v>0</v>
       </c>
-      <c r="AW9">
+      <c r="AW9" s="20">
         <v>11.764705882352942</v>
       </c>
-      <c r="AX9">
+      <c r="AX9" s="20">
         <v>5.882352941176471</v>
       </c>
-    </row>
-    <row r="10" spans="2:50" x14ac:dyDescent="0.25">
+      <c r="BV9" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="BW9" s="20">
+        <v>0</v>
+      </c>
+      <c r="BX9" s="20">
+        <v>0</v>
+      </c>
+      <c r="BY9" s="20">
+        <v>0</v>
+      </c>
+      <c r="BZ9" s="20">
+        <v>0</v>
+      </c>
+      <c r="CA9" s="20">
+        <v>23.529411764705884</v>
+      </c>
+      <c r="CB9" s="20">
+        <v>76.470588235294116</v>
+      </c>
+    </row>
+    <row r="10" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>5</v>
       </c>
@@ -13571,29 +15234,50 @@
       <c r="AJ10" s="3">
         <v>88.235294117647058</v>
       </c>
-      <c r="AR10" t="s">
+      <c r="AR10" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="AS10">
+      <c r="AS10" s="20">
         <v>-5.882352941176471</v>
       </c>
-      <c r="AT10">
+      <c r="AT10" s="20">
         <v>0</v>
       </c>
-      <c r="AU10">
+      <c r="AU10" s="20">
         <v>-5.882352941176471</v>
       </c>
-      <c r="AV10">
+      <c r="AV10" s="20">
         <v>5.882352941176471</v>
       </c>
-      <c r="AW10">
+      <c r="AW10" s="20">
         <v>29.411764705882351</v>
       </c>
-      <c r="AX10">
+      <c r="AX10" s="20">
         <v>52.941176470588232</v>
       </c>
-    </row>
-    <row r="11" spans="2:50" x14ac:dyDescent="0.25">
+      <c r="BV10" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="BW10" s="20">
+        <v>-70.588235294117652</v>
+      </c>
+      <c r="BX10" s="20">
+        <v>-23.529411764705884</v>
+      </c>
+      <c r="BY10" s="20">
+        <v>-2.9411764705882355</v>
+      </c>
+      <c r="BZ10" s="20">
+        <v>2.9411764705882355</v>
+      </c>
+      <c r="CA10" s="20">
+        <v>0</v>
+      </c>
+      <c r="CB10" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>4</v>
       </c>
@@ -13645,29 +15329,50 @@
       <c r="AJ11" s="3">
         <v>0</v>
       </c>
-      <c r="AR11" t="s">
+      <c r="AR11" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="AS11">
+      <c r="AS11" s="20">
         <v>0</v>
       </c>
-      <c r="AT11">
+      <c r="AT11" s="20">
         <v>-23.529411764705884</v>
       </c>
-      <c r="AU11">
+      <c r="AU11" s="20">
         <v>-64.705882352941174</v>
       </c>
-      <c r="AV11">
+      <c r="AV11" s="20">
         <v>0</v>
       </c>
-      <c r="AW11">
+      <c r="AW11" s="20">
         <v>11.764705882352942</v>
       </c>
-      <c r="AX11">
+      <c r="AX11" s="20">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:50" x14ac:dyDescent="0.25">
+      <c r="BV11" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BW11" s="20">
+        <v>0</v>
+      </c>
+      <c r="BX11" s="20">
+        <v>0</v>
+      </c>
+      <c r="BY11" s="20">
+        <v>0</v>
+      </c>
+      <c r="BZ11" s="20">
+        <v>0</v>
+      </c>
+      <c r="CA11" s="20">
+        <v>11.764705882352942</v>
+      </c>
+      <c r="CB11" s="20">
+        <v>88.235294117647058</v>
+      </c>
+    </row>
+    <row r="12" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>5</v>
       </c>
@@ -13698,29 +15403,50 @@
       <c r="K12">
         <v>1</v>
       </c>
-      <c r="AR12" t="s">
+      <c r="AR12" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="AS12">
+      <c r="AS12" s="20">
         <v>0</v>
       </c>
-      <c r="AT12">
+      <c r="AT12" s="20">
         <v>0</v>
       </c>
-      <c r="AU12">
+      <c r="AU12" s="20">
         <v>0</v>
       </c>
-      <c r="AV12">
+      <c r="AV12" s="20">
         <v>0</v>
       </c>
-      <c r="AW12">
+      <c r="AW12" s="20">
         <v>23.529411764705884</v>
       </c>
-      <c r="AX12">
+      <c r="AX12" s="20">
         <v>76.470588235294116</v>
       </c>
-    </row>
-    <row r="13" spans="2:50" x14ac:dyDescent="0.25">
+      <c r="BV12" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="BW12" s="20">
+        <v>-76.470588235294116</v>
+      </c>
+      <c r="BX12" s="20">
+        <v>-17.647058823529413</v>
+      </c>
+      <c r="BY12" s="20">
+        <v>0</v>
+      </c>
+      <c r="BZ12" s="20">
+        <v>0</v>
+      </c>
+      <c r="CA12" s="20">
+        <v>5.882352941176471</v>
+      </c>
+      <c r="CB12" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>4</v>
       </c>
@@ -13803,29 +15529,29 @@
       <c r="AJ13" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="AR13" t="s">
+      <c r="AR13" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="AS13">
+      <c r="AS13" s="20">
         <v>-2.9411764705882355</v>
       </c>
-      <c r="AT13">
+      <c r="AT13" s="20">
         <v>-23.529411764705884</v>
       </c>
-      <c r="AU13">
+      <c r="AU13" s="20">
         <v>-70.588235294117652</v>
       </c>
-      <c r="AV13">
+      <c r="AV13" s="20">
         <v>2.9411764705882355</v>
       </c>
-      <c r="AW13">
+      <c r="AW13" s="20">
         <v>0</v>
       </c>
-      <c r="AX13">
+      <c r="AX13" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>3</v>
       </c>
@@ -13914,29 +15640,29 @@
       <c r="AJ14" s="7">
         <v>35.294117647058826</v>
       </c>
-      <c r="AR14" t="s">
+      <c r="AR14" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="AS14">
+      <c r="AS14" s="20">
         <v>0</v>
       </c>
-      <c r="AT14">
+      <c r="AT14" s="20">
         <v>0</v>
       </c>
-      <c r="AU14">
+      <c r="AU14" s="20">
         <v>0</v>
       </c>
-      <c r="AV14">
+      <c r="AV14" s="20">
         <v>0</v>
       </c>
-      <c r="AW14">
+      <c r="AW14" s="20">
         <v>11.764705882352942</v>
       </c>
-      <c r="AX14">
+      <c r="AX14" s="20">
         <v>88.235294117647058</v>
       </c>
     </row>
-    <row r="15" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>4</v>
       </c>
@@ -14025,29 +15751,29 @@
       <c r="AJ15" s="7">
         <v>0</v>
       </c>
-      <c r="AR15" t="s">
+      <c r="AR15" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="AS15">
+      <c r="AS15" s="20">
         <v>0</v>
       </c>
-      <c r="AT15">
+      <c r="AT15" s="20">
         <v>-17.647058823529413</v>
       </c>
-      <c r="AU15">
+      <c r="AU15" s="20">
         <v>-76.470588235294116</v>
       </c>
-      <c r="AV15">
+      <c r="AV15" s="20">
         <v>0</v>
       </c>
-      <c r="AW15">
+      <c r="AW15" s="20">
         <v>5.882352941176471</v>
       </c>
-      <c r="AX15">
+      <c r="AX15" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:50" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>5</v>
       </c>
@@ -14607,7 +16333,7 @@
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15063,7 +16789,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15914,14 +17640,57 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F62C60-52E5-48D1-8EE3-DA050404E753}">
-  <dimension ref="A3:X25"/>
+  <dimension ref="A2:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+      <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="11.7109375" customWidth="1"/>
+    <col min="23" max="23" width="23.28515625" customWidth="1"/>
+    <col min="24" max="24" width="13.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>165</v>
+      </c>
+      <c r="N2" t="s">
+        <v>166</v>
+      </c>
+      <c r="O2" t="s">
+        <v>167</v>
+      </c>
+      <c r="P2" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>169</v>
+      </c>
+      <c r="R2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" t="s">
+        <v>170</v>
+      </c>
+      <c r="T2" t="s">
+        <v>171</v>
+      </c>
+      <c r="U2" t="s">
+        <v>172</v>
+      </c>
+      <c r="V2" t="s">
+        <v>17</v>
+      </c>
+      <c r="W2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X2" t="s">
+        <v>173</v>
+      </c>
+    </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
@@ -17334,6 +19103,9 @@
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>174</v>
+      </c>
       <c r="N20">
         <f>_xlfn.VAR.P(N3:N19)</f>
         <v>0.69204152249134943</v>
@@ -17376,29 +19148,42 @@
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W22" t="s">
+        <v>161</v>
+      </c>
       <c r="X22">
         <f>SUM(N20:W20)</f>
         <v>5.8892733564013842</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W23" t="s">
+        <v>163</v>
+      </c>
       <c r="X23">
         <f>_xlfn.VAR.P(X3:X19)</f>
         <v>16.484429065743946</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W24" t="s">
+        <v>162</v>
+      </c>
       <c r="X24">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W25" t="s">
+        <v>164</v>
+      </c>
       <c r="X25">
         <f>(10/(10-1))*(1-(X22/X23))</f>
         <v>0.71415243959324581</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Exergame adaptation loop simulation
</commit_message>
<xml_diff>
--- a/data/Wearable Inertial Sensors for Exergames (post survey)_August 31, 2019_11.58.xlsx
+++ b/data/Wearable Inertial Sensors for Exergames (post survey)_August 31, 2019_11.58.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\github\wearable-jacket\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF11F825-D8E2-4B4D-B1AF-CA3F00884BBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E91DFA2-AE25-4A5D-8235-0F87EC7D2C1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="612" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="612" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wearable Inertial Sensors for E" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="175">
   <si>
     <t>StartDate</t>
   </si>
@@ -1120,7 +1120,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1163,13 +1163,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1305,7 +1299,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0EE18808-2F9A-4EBC-80A2-5AB9E45E94AA}" type="CELLRANGE">
+                    <a:fld id="{2D8AA33A-EC0A-429F-AE46-AFF1AF1FAC41}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1357,7 +1351,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1391,7 +1384,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1425,7 +1417,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1446,7 +1437,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2DC3080C-CB4C-427E-B5A3-5C212209E818}" type="CELLRANGE">
+                    <a:fld id="{E7E2E1CC-0F1F-4CFC-8DAA-061E1F359C82}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1498,7 +1489,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1532,7 +1522,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1553,7 +1542,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{055E07E0-8347-425D-A3FC-D54402F68DFE}" type="CELLRANGE">
+                    <a:fld id="{94A473F4-7B57-4D82-8A6D-8BCAA944247C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1605,7 +1594,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1639,7 +1627,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1871,7 +1858,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B35974E9-ACA2-4C5A-9C6A-4009B8DD35EA}" type="CELLRANGE">
+                    <a:fld id="{F062A901-5F23-471B-981B-C1438504A7D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1924,7 +1911,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1939,7 +1925,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{23116A68-313B-423C-94D5-1835928376BA}" type="CELLRANGE">
+                    <a:fld id="{C0DA4C5E-4716-4584-AEDE-9B2B79545A4B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1973,7 +1959,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB710C7B-E5A3-452B-9CD3-532F61038CA2}" type="CELLRANGE">
+                    <a:fld id="{6E335A81-4785-4BC1-803F-A7B8DB9E2960}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2007,7 +1993,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CDCA02FE-BA9C-42A3-A79B-121B990E7C83}" type="CELLRANGE">
+                    <a:fld id="{91474AA8-0CF9-49F7-B69B-0F0549C71379}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2060,7 +2046,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2075,7 +2060,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{69FBE8F8-5C2A-406A-A27F-FE20DF8C10FE}" type="CELLRANGE">
+                    <a:fld id="{F110C36C-248D-4470-BCAF-5AAFE010E5AC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2128,7 +2113,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2143,7 +2127,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8788A963-F285-4868-B4DD-9DC898E52864}" type="CELLRANGE">
+                    <a:fld id="{98AFD070-C1BB-40F1-B808-C4ACC2937B08}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2370,7 +2354,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3BD1EEF2-2745-45E3-AFE3-4B6BFA076509}" type="CELLRANGE">
+                    <a:fld id="{B5782981-BC1A-425E-86BF-97631E65260D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2404,7 +2388,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{553864B7-533D-47CD-9C9C-56616163EEFD}" type="CELLRANGE">
+                    <a:fld id="{7611FF54-3414-4524-ADE7-8B07F6BCA201}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2457,7 +2441,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2472,7 +2455,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EA8C31DD-5694-476F-BB2B-64D1C98CECD1}" type="CELLRANGE">
+                    <a:fld id="{CFB1CB13-D9BF-4EBD-BAEE-F68DE404FC27}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2525,7 +2508,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2540,7 +2522,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD280660-8009-449F-836B-4AC10E1E6C04}" type="CELLRANGE">
+                    <a:fld id="{E632DF35-2833-4F6B-A766-46327B6939E8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2593,7 +2575,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2608,7 +2589,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7F35CB66-412D-47E5-A5C9-BCBE59B96EB6}" type="CELLRANGE">
+                    <a:fld id="{07A223A0-3D9F-40B0-AA3D-A0864926F00C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2661,7 +2642,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2676,7 +2656,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F1D3B5D-362A-4032-B5D4-79BB62294558}" type="CELLRANGE">
+                    <a:fld id="{4FBB0C05-5646-46AB-8951-783A035F96CF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3010,7 +2990,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{72FBFEC3-7771-4536-842E-5A084DA281E2}" type="CELLRANGE">
+                    <a:fld id="{A5F59C8B-0D80-4351-954D-D2B93E52164C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3063,7 +3043,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -3078,7 +3057,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1B6F112B-86CC-4573-909B-36F83EBB5293}" type="CELLRANGE">
+                    <a:fld id="{9FBAAE9A-F213-49B9-98A3-604F9EEA8D9D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3112,7 +3091,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{424285C5-F7D6-4B10-B9D5-D292FC53C554}" type="CELLRANGE">
+                    <a:fld id="{F84CB238-E347-4116-827A-49D74D9909E5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3146,7 +3125,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D23FAFC4-956A-482A-8C9C-44917C28CD3F}" type="CELLRANGE">
+                    <a:fld id="{7B2982FE-3188-4092-9798-2E3425A802D2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3180,7 +3159,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{428FF211-1B59-4E79-A384-7987E8E951BE}" type="CELLRANGE">
+                    <a:fld id="{F1C9D83E-E54C-44ED-84DA-63ECEB46D252}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3214,7 +3193,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D84AFA1D-EDF4-43BC-84D2-A5E94441706E}" type="CELLRANGE">
+                    <a:fld id="{70F0A7BE-1470-4378-98DB-540B02A6A54C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3267,7 +3246,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -3282,7 +3260,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B3B4728-FB1D-4122-B95C-AFEF3DE483DA}" type="CELLRANGE">
+                    <a:fld id="{44FA2339-97B8-4131-A94D-E54F70E92A0B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3316,7 +3294,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BE70C978-4873-484E-B6C1-0A48F2171FB6}" type="CELLRANGE">
+                    <a:fld id="{21432433-D2AF-4065-BE06-9F084B0D0821}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3549,7 +3527,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{07C887BA-733C-4A19-A5CD-9C7C8605602D}" type="CELLRANGE">
+                    <a:fld id="{D2016F2A-1CCC-41EB-900F-A0109B2FF0CA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3602,7 +3580,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -3617,7 +3594,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B431E305-2443-496D-9F82-86648684E24F}" type="CELLRANGE">
+                    <a:fld id="{2DC2CC9F-0240-4C66-820C-A8595751C787}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3651,7 +3628,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{471B020D-82A3-4F20-B572-73D289D59AEE}" type="CELLRANGE">
+                    <a:fld id="{57D59CB8-2B6F-4939-BF68-107541CF17A5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3685,7 +3662,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{17BA4E8A-CC2A-4DFD-9B55-EA627A90830B}" type="CELLRANGE">
+                    <a:fld id="{AECD1BE4-856D-42D1-895E-16B8737C083F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3738,7 +3715,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -3753,7 +3729,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F47326D2-D875-4770-88CE-07804168A4C9}" type="CELLRANGE">
+                    <a:fld id="{96DD96FA-1B6F-4929-AE98-CAC32C3B6F2D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3806,7 +3782,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -3821,7 +3796,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{44EA7E48-6F8A-497B-B34F-B383DE80A765}" type="CELLRANGE">
+                    <a:fld id="{154C5446-C2A3-4C9E-BFB7-E230BE8027BE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3874,7 +3849,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -8613,716 +8587,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Picture 24">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3BE8954-6F1C-40C3-B16D-94380C5768D5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="5400675"/>
-          <a:ext cx="381000" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Picture 25">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47DA7031-ED66-4388-B827-C7AB08CB28D8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="5781675"/>
-          <a:ext cx="400050" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Picture 26">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07C31B4D-19FD-4963-B653-D22A4BD48E2C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="6162675"/>
-          <a:ext cx="361950" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Picture 27">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B81C5A1-732C-4FCB-86D0-D845D85EB13E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="6543675"/>
-          <a:ext cx="457200" cy="209550"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="Picture 28">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE371D02-2CC1-4C6B-998C-FAB9A60DB272}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="6924675"/>
-          <a:ext cx="457200" cy="209550"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Picture 29">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78FACE58-E24C-45C5-8B58-CF93AAAB26A3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="7305675"/>
-          <a:ext cx="390525" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="Picture 30">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2B958AB-BF7B-4BB9-8BEF-CE353753BFFB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="7686675"/>
-          <a:ext cx="409575" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="32" name="Picture 31">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4BB989F-E2A1-4511-8A6B-3E92C1E8AF3B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="8067675"/>
-          <a:ext cx="371475" cy="180975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="Picture 32">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D52DA72D-0A6A-40A9-8D79-A593C8D59E25}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="8448675"/>
-          <a:ext cx="466725" cy="209550"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="Picture 33">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D54F85AC-B3E7-4A4D-9FEE-17238ECF3C3A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="8829675"/>
-          <a:ext cx="466725" cy="209550"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -14386,22 +13650,22 @@
       <c r="BV3" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="BW3" s="20">
+      <c r="BW3" s="18">
         <v>0</v>
       </c>
-      <c r="BX3" s="20">
+      <c r="BX3" s="18">
         <v>-5.882352941176471</v>
       </c>
-      <c r="BY3" s="20">
+      <c r="BY3" s="18">
         <v>-5.882352941176471</v>
       </c>
-      <c r="BZ3" s="20">
+      <c r="BZ3" s="18">
         <v>5.882352941176471</v>
       </c>
-      <c r="CA3" s="20">
+      <c r="CA3" s="18">
         <v>47.058823529411768</v>
       </c>
-      <c r="CB3" s="20">
+      <c r="CB3" s="18">
         <v>35.294117647058826</v>
       </c>
     </row>
@@ -14506,22 +13770,22 @@
       <c r="BV4" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="BW4" s="20">
+      <c r="BW4" s="18">
         <v>-76.470588235294116</v>
       </c>
-      <c r="BX4" s="20">
+      <c r="BX4" s="18">
         <v>-23.529411764705884</v>
       </c>
-      <c r="BY4" s="20">
+      <c r="BY4" s="18">
         <v>0</v>
       </c>
-      <c r="BZ4" s="20">
+      <c r="BZ4" s="18">
         <v>0</v>
       </c>
-      <c r="CA4" s="20">
+      <c r="CA4" s="18">
         <v>0</v>
       </c>
-      <c r="CB4" s="20">
+      <c r="CB4" s="18">
         <v>0</v>
       </c>
     </row>
@@ -14645,22 +13909,22 @@
       <c r="BV5" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="BW5" s="20">
+      <c r="BW5" s="18">
         <v>0</v>
       </c>
-      <c r="BX5" s="20">
+      <c r="BX5" s="18">
         <v>0</v>
       </c>
-      <c r="BY5" s="20">
+      <c r="BY5" s="18">
         <v>0</v>
       </c>
-      <c r="BZ5" s="20">
+      <c r="BZ5" s="18">
         <v>0</v>
       </c>
-      <c r="CA5" s="20">
+      <c r="CA5" s="18">
         <v>17.647058823529413</v>
       </c>
-      <c r="CB5" s="20">
+      <c r="CB5" s="18">
         <v>82.352941176470594</v>
       </c>
     </row>
@@ -14765,43 +14029,43 @@
       <c r="AR6" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="AS6" s="20">
+      <c r="AS6" s="18">
         <v>-5.882352941176471</v>
       </c>
-      <c r="AT6" s="20">
+      <c r="AT6" s="18">
         <v>-5.882352941176471</v>
       </c>
-      <c r="AU6" s="20">
+      <c r="AU6" s="18">
         <v>0</v>
       </c>
-      <c r="AV6" s="20">
+      <c r="AV6" s="18">
         <v>5.882352941176471</v>
       </c>
-      <c r="AW6" s="20">
+      <c r="AW6" s="18">
         <v>47.058823529411768</v>
       </c>
-      <c r="AX6" s="20">
+      <c r="AX6" s="18">
         <v>35.294117647058826</v>
       </c>
       <c r="BV6" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="BW6" s="20">
+      <c r="BW6" s="18">
         <v>-64.705882352941174</v>
       </c>
-      <c r="BX6" s="20">
+      <c r="BX6" s="18">
         <v>-17.647058823529413</v>
       </c>
-      <c r="BY6" s="20">
+      <c r="BY6" s="18">
         <v>0</v>
       </c>
-      <c r="BZ6" s="20">
+      <c r="BZ6" s="18">
         <v>0</v>
       </c>
-      <c r="CA6" s="20">
+      <c r="CA6" s="18">
         <v>11.764705882352942</v>
       </c>
-      <c r="CB6" s="20">
+      <c r="CB6" s="18">
         <v>5.882352941176471</v>
       </c>
     </row>
@@ -14906,43 +14170,43 @@
       <c r="AR7" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="AS7" s="20">
+      <c r="AS7" s="18">
         <v>0</v>
       </c>
-      <c r="AT7" s="20">
+      <c r="AT7" s="18">
         <v>-23.529411764705884</v>
       </c>
-      <c r="AU7" s="20">
+      <c r="AU7" s="18">
         <v>-76.470588235294116</v>
       </c>
-      <c r="AV7" s="20">
+      <c r="AV7" s="18">
         <v>0</v>
       </c>
-      <c r="AW7" s="20">
+      <c r="AW7" s="18">
         <v>0</v>
       </c>
-      <c r="AX7" s="20">
+      <c r="AX7" s="18">
         <v>0</v>
       </c>
       <c r="BV7" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="BW7" s="20">
+      <c r="BW7" s="18">
         <v>-5.882352941176471</v>
       </c>
-      <c r="BX7" s="20">
+      <c r="BX7" s="18">
         <v>0</v>
       </c>
-      <c r="BY7" s="20">
+      <c r="BY7" s="18">
         <v>-5.882352941176471</v>
       </c>
-      <c r="BZ7" s="20">
+      <c r="BZ7" s="18">
         <v>5.882352941176471</v>
       </c>
-      <c r="CA7" s="20">
+      <c r="CA7" s="18">
         <v>29.411764705882351</v>
       </c>
-      <c r="CB7" s="20">
+      <c r="CB7" s="18">
         <v>52.941176470588232</v>
       </c>
     </row>
@@ -15047,43 +14311,43 @@
       <c r="AR8" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="AS8" s="20">
+      <c r="AS8" s="18">
         <v>0</v>
       </c>
-      <c r="AT8" s="20">
+      <c r="AT8" s="18">
         <v>0</v>
       </c>
-      <c r="AU8" s="20">
+      <c r="AU8" s="18">
         <v>0</v>
       </c>
-      <c r="AV8" s="20">
+      <c r="AV8" s="18">
         <v>0</v>
       </c>
-      <c r="AW8" s="20">
+      <c r="AW8" s="18">
         <v>17.647058823529413</v>
       </c>
-      <c r="AX8" s="20">
+      <c r="AX8" s="18">
         <v>82.352941176470594</v>
       </c>
       <c r="BV8" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="BW8" s="20">
+      <c r="BW8" s="18">
         <v>-64.705882352941174</v>
       </c>
-      <c r="BX8" s="20">
+      <c r="BX8" s="18">
         <v>-23.529411764705884</v>
       </c>
-      <c r="BY8" s="20">
+      <c r="BY8" s="18">
         <v>0</v>
       </c>
-      <c r="BZ8" s="20">
+      <c r="BZ8" s="18">
         <v>0</v>
       </c>
-      <c r="CA8" s="20">
+      <c r="CA8" s="18">
         <v>11.764705882352942</v>
       </c>
-      <c r="CB8" s="20">
+      <c r="CB8" s="18">
         <v>0</v>
       </c>
     </row>
@@ -15142,43 +14406,43 @@
       <c r="AR9" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="AS9" s="20">
+      <c r="AS9" s="18">
         <v>0</v>
       </c>
-      <c r="AT9" s="20">
+      <c r="AT9" s="18">
         <v>-17.647058823529413</v>
       </c>
-      <c r="AU9" s="20">
+      <c r="AU9" s="18">
         <v>-64.705882352941174</v>
       </c>
-      <c r="AV9" s="20">
+      <c r="AV9" s="18">
         <v>0</v>
       </c>
-      <c r="AW9" s="20">
+      <c r="AW9" s="18">
         <v>11.764705882352942</v>
       </c>
-      <c r="AX9" s="20">
+      <c r="AX9" s="18">
         <v>5.882352941176471</v>
       </c>
       <c r="BV9" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="BW9" s="20">
+      <c r="BW9" s="18">
         <v>0</v>
       </c>
-      <c r="BX9" s="20">
+      <c r="BX9" s="18">
         <v>0</v>
       </c>
-      <c r="BY9" s="20">
+      <c r="BY9" s="18">
         <v>0</v>
       </c>
-      <c r="BZ9" s="20">
+      <c r="BZ9" s="18">
         <v>0</v>
       </c>
-      <c r="CA9" s="20">
+      <c r="CA9" s="18">
         <v>23.529411764705884</v>
       </c>
-      <c r="CB9" s="20">
+      <c r="CB9" s="18">
         <v>76.470588235294116</v>
       </c>
     </row>
@@ -15237,43 +14501,43 @@
       <c r="AR10" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="AS10" s="20">
+      <c r="AS10" s="18">
         <v>-5.882352941176471</v>
       </c>
-      <c r="AT10" s="20">
+      <c r="AT10" s="18">
         <v>0</v>
       </c>
-      <c r="AU10" s="20">
+      <c r="AU10" s="18">
         <v>-5.882352941176471</v>
       </c>
-      <c r="AV10" s="20">
+      <c r="AV10" s="18">
         <v>5.882352941176471</v>
       </c>
-      <c r="AW10" s="20">
+      <c r="AW10" s="18">
         <v>29.411764705882351</v>
       </c>
-      <c r="AX10" s="20">
+      <c r="AX10" s="18">
         <v>52.941176470588232</v>
       </c>
       <c r="BV10" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="BW10" s="20">
+      <c r="BW10" s="18">
         <v>-70.588235294117652</v>
       </c>
-      <c r="BX10" s="20">
+      <c r="BX10" s="18">
         <v>-23.529411764705884</v>
       </c>
-      <c r="BY10" s="20">
+      <c r="BY10" s="18">
         <v>-2.9411764705882355</v>
       </c>
-      <c r="BZ10" s="20">
+      <c r="BZ10" s="18">
         <v>2.9411764705882355</v>
       </c>
-      <c r="CA10" s="20">
+      <c r="CA10" s="18">
         <v>0</v>
       </c>
-      <c r="CB10" s="20">
+      <c r="CB10" s="18">
         <v>0</v>
       </c>
     </row>
@@ -15332,43 +14596,43 @@
       <c r="AR11" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="AS11" s="20">
+      <c r="AS11" s="18">
         <v>0</v>
       </c>
-      <c r="AT11" s="20">
+      <c r="AT11" s="18">
         <v>-23.529411764705884</v>
       </c>
-      <c r="AU11" s="20">
+      <c r="AU11" s="18">
         <v>-64.705882352941174</v>
       </c>
-      <c r="AV11" s="20">
+      <c r="AV11" s="18">
         <v>0</v>
       </c>
-      <c r="AW11" s="20">
+      <c r="AW11" s="18">
         <v>11.764705882352942</v>
       </c>
-      <c r="AX11" s="20">
+      <c r="AX11" s="18">
         <v>0</v>
       </c>
       <c r="BV11" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="BW11" s="20">
+      <c r="BW11" s="18">
         <v>0</v>
       </c>
-      <c r="BX11" s="20">
+      <c r="BX11" s="18">
         <v>0</v>
       </c>
-      <c r="BY11" s="20">
+      <c r="BY11" s="18">
         <v>0</v>
       </c>
-      <c r="BZ11" s="20">
+      <c r="BZ11" s="18">
         <v>0</v>
       </c>
-      <c r="CA11" s="20">
+      <c r="CA11" s="18">
         <v>11.764705882352942</v>
       </c>
-      <c r="CB11" s="20">
+      <c r="CB11" s="18">
         <v>88.235294117647058</v>
       </c>
     </row>
@@ -15406,43 +14670,43 @@
       <c r="AR12" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="AS12" s="20">
+      <c r="AS12" s="18">
         <v>0</v>
       </c>
-      <c r="AT12" s="20">
+      <c r="AT12" s="18">
         <v>0</v>
       </c>
-      <c r="AU12" s="20">
+      <c r="AU12" s="18">
         <v>0</v>
       </c>
-      <c r="AV12" s="20">
+      <c r="AV12" s="18">
         <v>0</v>
       </c>
-      <c r="AW12" s="20">
+      <c r="AW12" s="18">
         <v>23.529411764705884</v>
       </c>
-      <c r="AX12" s="20">
+      <c r="AX12" s="18">
         <v>76.470588235294116</v>
       </c>
       <c r="BV12" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="BW12" s="20">
+      <c r="BW12" s="18">
         <v>-76.470588235294116</v>
       </c>
-      <c r="BX12" s="20">
+      <c r="BX12" s="18">
         <v>-17.647058823529413</v>
       </c>
-      <c r="BY12" s="20">
+      <c r="BY12" s="18">
         <v>0</v>
       </c>
-      <c r="BZ12" s="20">
+      <c r="BZ12" s="18">
         <v>0</v>
       </c>
-      <c r="CA12" s="20">
+      <c r="CA12" s="18">
         <v>5.882352941176471</v>
       </c>
-      <c r="CB12" s="20">
+      <c r="CB12" s="18">
         <v>0</v>
       </c>
     </row>
@@ -15532,22 +14796,22 @@
       <c r="AR13" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="AS13" s="20">
+      <c r="AS13" s="18">
         <v>-2.9411764705882355</v>
       </c>
-      <c r="AT13" s="20">
+      <c r="AT13" s="18">
         <v>-23.529411764705884</v>
       </c>
-      <c r="AU13" s="20">
+      <c r="AU13" s="18">
         <v>-70.588235294117652</v>
       </c>
-      <c r="AV13" s="20">
+      <c r="AV13" s="18">
         <v>2.9411764705882355</v>
       </c>
-      <c r="AW13" s="20">
+      <c r="AW13" s="18">
         <v>0</v>
       </c>
-      <c r="AX13" s="20">
+      <c r="AX13" s="18">
         <v>0</v>
       </c>
     </row>
@@ -15643,22 +14907,22 @@
       <c r="AR14" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="AS14" s="20">
+      <c r="AS14" s="18">
         <v>0</v>
       </c>
-      <c r="AT14" s="20">
+      <c r="AT14" s="18">
         <v>0</v>
       </c>
-      <c r="AU14" s="20">
+      <c r="AU14" s="18">
         <v>0</v>
       </c>
-      <c r="AV14" s="20">
+      <c r="AV14" s="18">
         <v>0</v>
       </c>
-      <c r="AW14" s="20">
+      <c r="AW14" s="18">
         <v>11.764705882352942</v>
       </c>
-      <c r="AX14" s="20">
+      <c r="AX14" s="18">
         <v>88.235294117647058</v>
       </c>
     </row>
@@ -15754,22 +15018,22 @@
       <c r="AR15" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="AS15" s="20">
+      <c r="AS15" s="18">
         <v>0</v>
       </c>
-      <c r="AT15" s="20">
+      <c r="AT15" s="18">
         <v>-17.647058823529413</v>
       </c>
-      <c r="AU15" s="20">
+      <c r="AU15" s="18">
         <v>-76.470588235294116</v>
       </c>
-      <c r="AV15" s="20">
+      <c r="AV15" s="18">
         <v>0</v>
       </c>
-      <c r="AW15" s="20">
+      <c r="AW15" s="18">
         <v>5.882352941176471</v>
       </c>
-      <c r="AX15" s="20">
+      <c r="AX15" s="18">
         <v>0</v>
       </c>
     </row>
@@ -16330,15 +15594,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8268C1A4-9360-4D70-A585-6E201842CAD7}">
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.7109375" customWidth="1"/>
+    <col min="1" max="1" width="45.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" customWidth="1"/>
     <col min="6" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -16355,7 +15619,7 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>147</v>
       </c>
       <c r="B2" s="12">
@@ -16645,142 +15909,10 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="16"/>
-    </row>
-    <row r="48" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="17" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="15" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="15" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="15" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="15" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="15" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="15" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
-        <v>156</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -16829,7 +15961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="19" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="17" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>46</v>
       </c>
@@ -17642,7 +16774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F62C60-52E5-48D1-8EE3-DA050404E753}">
   <dimension ref="A2:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>

</xml_diff>